<commit_message>
Update IP - EX 43 - Procv (Anexo).xlsx
Exercicio
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 43 - Procv (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 43 - Procv (Anexo).xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA454CA6-3A35-4E87-90F1-6A6358725F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2306B07-8B7C-457C-8EC0-4FB2D0CA7236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
     <sheet name="EXPLICAÇÃO" sheetId="4" r:id="rId2"/>
-    <sheet name="EXPLICAÇÃO (RESOLVIDO)" sheetId="7" state="hidden" r:id="rId3"/>
+    <sheet name="EXPLICAÇÃO (RESOLVIDO)" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2544" uniqueCount="150">
   <si>
     <t>PROCV</t>
   </si>
@@ -2065,7 +2065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -2242,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:R646"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,7 +2378,10 @@
       <c r="H11" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="46"/>
+      <c r="I11" s="46" t="str">
+        <f>VLOOKUP(B13,B12:D15,2,FALSE)</f>
+        <v>BANANA</v>
+      </c>
       <c r="K11" s="28"/>
     </row>
     <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2406,7 +2409,9 @@
       <c r="G13" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="65"/>
+      <c r="H13" s="65" t="s">
+        <v>10</v>
+      </c>
       <c r="I13" s="66"/>
     </row>
     <row r="14" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2433,7 +2438,10 @@
       <c r="H15" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="45"/>
+      <c r="I15" s="45" t="str">
+        <f>VLOOKUP(H13,B12:D15,2,)</f>
+        <v>MAÇA</v>
+      </c>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H16" s="44"/>
@@ -2442,7 +2450,10 @@
       <c r="H17" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="45"/>
+      <c r="I17" s="45" t="str">
+        <f>VLOOKUP(H13,B12:D15,3,FALSE)</f>
+        <v>VERMELHO</v>
+      </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="38" t="s">
@@ -2494,9 +2505,16 @@
       <c r="J20" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="65"/>
+      <c r="K20" s="65" t="s">
+        <v>4</v>
+      </c>
       <c r="L20" s="66"/>
-      <c r="N20" s="68"/>
+      <c r="N20" s="68" t="str">
+        <f>IF(VLOOKUP($K$20,$B$19:$G$24,6,FALSE)&lt;=K22,
+PROPER(K20) &amp; " está dentro do orçamento!",
+PROPER(K20) &amp; " passou orçamento por R$ " &amp; (VLOOKUP($K$20,$B$19:$G$24,6,FALSE)-K22) &amp; "!")</f>
+        <v>João passou orçamento por R$ 1000!</v>
+      </c>
       <c r="O20" s="69"/>
       <c r="P20" s="69"/>
       <c r="Q20" s="69"/>
@@ -2546,7 +2564,9 @@
       <c r="J22" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="K22" s="77"/>
+      <c r="K22" s="77">
+        <v>2000</v>
+      </c>
       <c r="L22" s="78"/>
       <c r="N22" s="74"/>
       <c r="O22" s="75"/>
@@ -2660,7 +2680,7 @@
         <v>41137</v>
       </c>
       <c r="J30" s="83">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="K30" s="84"/>
       <c r="L30" s="85"/>
@@ -2739,7 +2759,7 @@
         <v>41140</v>
       </c>
       <c r="J33" s="83" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K33" s="84"/>
       <c r="L33" s="85"/>
@@ -2847,7 +2867,10 @@
       <c r="H37" s="41">
         <v>41144</v>
       </c>
-      <c r="J37" s="63"/>
+      <c r="J37" s="63" t="str">
+        <f>VLOOKUP($J$30,$B$29:$H$646,MATCH($J$33,$B$29:$H$29,0),FALSE)</f>
+        <v>Pedro</v>
+      </c>
       <c r="K37" s="63"/>
       <c r="L37" s="63"/>
       <c r="M37" s="63"/>
@@ -3013,7 +3036,10 @@
       <c r="K43" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="L43" s="45"/>
+      <c r="L43" s="45" t="str">
+        <f>INDEX($B$30:$H$646,J30,MATCH(J33,B29:H29,0))</f>
+        <v>Pedro</v>
+      </c>
     </row>
     <row r="44" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="40">
@@ -16904,9 +16930,18 @@
     <mergeCell ref="J32:L32"/>
     <mergeCell ref="J33:L33"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K20:L20" xr:uid="{F5A9A3AF-C438-4F84-B1CA-B67CC4A4058B}">
       <formula1>$B$20:$B$24</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:I13" xr:uid="{145D7F43-51DD-4A12-A020-3CA8326DCBBE}">
+      <formula1>$B$13:$B$15</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J30:L30" xr:uid="{4346CDEE-675C-4D1A-9C7A-040187881E3B}">
+      <formula1>$B$30:$B$646</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J33:L33" xr:uid="{3F858E7C-B08D-40EA-BCBA-F690B3F9613D}">
+      <formula1>$C$29:$H$29</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -16926,7 +16961,7 @@
   <dimension ref="B2:Q626"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>